<commit_message>
Se actualiza la información del archivo que contiene la data de prueba
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/autRetoDatos.xlsx
+++ b/src/test/resources/DataDriven/autRetoDatos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5EBED9F-0483-417C-9981-6F733F81C1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62BDED72-A5A5-4CA0-8029-91B203355430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,31 +51,31 @@
     <t>contrasenausuario</t>
   </si>
   <si>
-    <t>Randy</t>
-  </si>
-  <si>
-    <t>Manu</t>
-  </si>
-  <si>
-    <t>Ospina</t>
-  </si>
-  <si>
-    <t>RanMa01</t>
+    <t>Monica</t>
+  </si>
+  <si>
+    <t>Francisca</t>
+  </si>
+  <si>
+    <t>Gastanbide</t>
+  </si>
+  <si>
+    <t>MonicaF1</t>
   </si>
   <si>
     <t>123434.aeiuy</t>
   </si>
   <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Sebastian</t>
-  </si>
-  <si>
-    <t>Correa Orosco</t>
-  </si>
-  <si>
-    <t>JoSeC01</t>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Lecrec Montez</t>
+  </si>
+  <si>
+    <t>CharlesAL112</t>
   </si>
   <si>
     <t>contrasena_12</t>
@@ -453,7 +453,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -497,7 +497,7 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>2025240710</v>
+        <v>2025240810</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -517,7 +517,7 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>2025240711</v>
+        <v>2025240811</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Se realiza mejoras al codigo y se cambia la información de la data de pruebas
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/autRetoDatos.xlsx
+++ b/src/test/resources/DataDriven/autRetoDatos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62BDED72-A5A5-4CA0-8029-91B203355430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB80DE71-A23A-40E4-AF48-AF5C685AB8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,31 +51,31 @@
     <t>contrasenausuario</t>
   </si>
   <si>
-    <t>Monica</t>
-  </si>
-  <si>
-    <t>Francisca</t>
-  </si>
-  <si>
-    <t>Gastanbide</t>
-  </si>
-  <si>
-    <t>MonicaF1</t>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Verstapen</t>
+  </si>
+  <si>
+    <t>Quimera</t>
+  </si>
+  <si>
+    <t>MaxF1V</t>
   </si>
   <si>
     <t>123434.aeiuy</t>
   </si>
   <si>
-    <t>Charles</t>
-  </si>
-  <si>
-    <t>Antonio</t>
-  </si>
-  <si>
-    <t>Lecrec Montez</t>
-  </si>
-  <si>
-    <t>CharlesAL112</t>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>Hamilton Vera</t>
+  </si>
+  <si>
+    <t>LHalF1</t>
   </si>
   <si>
     <t>contrasena_12</t>
@@ -460,7 +460,7 @@
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
@@ -497,7 +497,7 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>2025240810</v>
+        <v>202102001</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -517,7 +517,7 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>2025240811</v>
+        <v>202102002</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>

</xml_diff>